<commit_message>
Succesfully Merged appended Parallel downloads
</commit_message>
<xml_diff>
--- a/user_input/twitter_users.xlsx
+++ b/user_input/twitter_users.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Public_Github\Social_Media\Social_Media_Pipeline\user_input\test\small\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Public_Github\Social_Media\Social_Media_Pipeline\user_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D48E7CF-AABB-4C69-9922-C7D66822D802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED00F22A-7016-4902-9511-9159ED48097A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5448" yWindow="2196" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,9 +123,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <gradientFill degree="135">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="4"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="135">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="4"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="135">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="4"/>
+          </stop>
+        </gradientFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -158,42 +191,6 @@
     </dxf>
     <dxf>
       <fill>
-        <gradientFill degree="135">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="4"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="135">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="4"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="135">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="4"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor theme="0"/>
@@ -225,12 +222,12 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="PivotTable Style 1" table="0" count="1" xr9:uid="{3E1625D2-EEB8-4646-8733-FB34F1DD13C7}">
-      <tableStyleElement type="firstRowStripe" dxfId="10"/>
+      <tableStyleElement type="firstRowStripe" dxfId="9"/>
     </tableStyle>
     <tableStyle name="Table Style 1" pivot="0" count="3" xr9:uid="{B0C9802B-C3E9-40BC-823C-C4F0238421C7}">
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="firstRowStripe" dxfId="8"/>
-      <tableStyleElement type="secondRowStripe" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="secondRowStripe" dxfId="6"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -258,11 +255,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{533D40E5-BD8F-4694-ABE3-333B2EFC261C}" name="Table2" displayName="Table2" ref="A1:B24" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2">
-  <autoFilter ref="A1:B24" xr:uid="{533D40E5-BD8F-4694-ABE3-333B2EFC261C}"/>
-  <tableColumns count="2">
-    <tableColumn id="6" xr3:uid="{6588CB0A-19DB-4E8A-9A90-B3DE13D8D1FD}" name="US_journals" dataDxfId="1"/>
-    <tableColumn id="1" xr3:uid="{6C89AA30-D463-4BC4-A11D-75D3873B8FD4}" name="international_news" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{533D40E5-BD8F-4694-ABE3-333B2EFC261C}" name="Table2" displayName="Table2" ref="A1:A24" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4">
+  <autoFilter ref="A1:A24" xr:uid="{533D40E5-BD8F-4694-ABE3-333B2EFC261C}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{6C89AA30-D463-4BC4-A11D-75D3873B8FD4}" name="international_news" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -593,38 +589,38 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
@@ -708,19 +704,19 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:A24">
-    <cfRule type="containsBlanks" dxfId="6" priority="3">
+  <conditionalFormatting sqref="B2:B24">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(B2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A4">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B4">
-    <cfRule type="containsBlanks" dxfId="5" priority="2">
-      <formula>LEN(TRIM(B2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:B24">
-    <cfRule type="containsBlanks" dxfId="4" priority="1">
-      <formula>LEN(TRIM(B5))=0</formula>
+  <conditionalFormatting sqref="A5:A24">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(A5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>